<commit_message>
export schedule/staff after modify
</commit_message>
<xml_diff>
--- a/staff.xlsx
+++ b/staff.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>ID</t>
   </si>
@@ -35,6 +35,24 @@
   </si>
   <si>
     <t>Theater</t>
+  </si>
+  <si>
+    <t>Emily Galaxy</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Art</t>
+  </si>
+  <si>
+    <t>Lucas Luna</t>
+  </si>
+  <si>
+    <t>Adam Justin</t>
+  </si>
+  <si>
+    <t>Dance</t>
   </si>
 </sst>
 </file>
@@ -375,7 +393,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -412,6 +430,48 @@
         <v>6</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>